<commit_message>
filling in pizza example
</commit_message>
<xml_diff>
--- a/notebooks/pizza-lp/pizza-lp.xlsx
+++ b/notebooks/pizza-lp/pizza-lp.xlsx
@@ -1,64 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbiagion/gitrepos/optimization-modeling-info-3440/notebooks/pizza-lp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave.Biagioni\gitrepos\optimization-modeling-info-3440\notebooks\pizza-lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7679A24-F0E2-434F-B05C-63C41B409E0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34300" yWindow="-7020" windowWidth="28780" windowHeight="14260" xr2:uid="{8EB81697-7FD5-9F49-8C1E-BED112DAE188}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="2.2" sheetId="2" r:id="rId1"/>
-    <sheet name="6.5" sheetId="3" r:id="rId2"/>
+    <sheet name="profit" sheetId="7" r:id="rId2"/>
+    <sheet name="resource" sheetId="8" r:id="rId3"/>
+    <sheet name="rhs" sheetId="9" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'6.5'!$C$12:$J$12</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'6.5'!$C$12:$J$12</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'6.5'!$C$19:$C$21</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'6.5'!$C$22</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'6.5'!$C$22</definedName>
-    <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'6.5'!$C$14</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">5</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">binary</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'6.5'!$E$19:$E$21</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'6.5'!$E$22</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'6.5'!$E$22</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Decision variables (pizza types)</t>
   </si>
@@ -120,85 +79,25 @@
     <t>veggies</t>
   </si>
   <si>
-    <t xml:space="preserve">Data </t>
-  </si>
-  <si>
-    <t>Number of available scientists</t>
-  </si>
-  <si>
-    <t>Available budget</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Expense ($000)</t>
-  </si>
-  <si>
-    <t>Scientists Required</t>
-  </si>
-  <si>
-    <t>Profit ($000)</t>
-  </si>
-  <si>
-    <t>Decisions</t>
-  </si>
-  <si>
-    <t>Project 1</t>
-  </si>
-  <si>
-    <t>Project 2</t>
-  </si>
-  <si>
-    <t>Project 3</t>
-  </si>
-  <si>
-    <t>Project 4</t>
-  </si>
-  <si>
-    <t>Project 5</t>
-  </si>
-  <si>
-    <t>Project 6</t>
-  </si>
-  <si>
-    <t>Project 7</t>
-  </si>
-  <si>
-    <t>Project 8</t>
-  </si>
-  <si>
-    <t>Objective:  Maximize profit</t>
-  </si>
-  <si>
-    <t>Binary decisions</t>
-  </si>
-  <si>
-    <t>(see Solver)</t>
-  </si>
-  <si>
-    <t>Expenses must be within budget</t>
-  </si>
-  <si>
-    <t>Either 2 or 5 but not both</t>
-  </si>
-  <si>
-    <t>At least 2 of proj. 5-8</t>
-  </si>
-  <si>
-    <t>&gt;=</t>
-  </si>
-  <si>
     <t>slack</t>
   </si>
   <si>
-    <t>Scientists must be within budget</t>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>pizza</t>
+  </si>
+  <si>
+    <t>rhs</t>
+  </si>
+  <si>
+    <t>resource</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -258,21 +157,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Currency 2" xfId="2" xr:uid="{998F847E-5BC8-7741-A5AD-CF273087D315}"/>
+    <cellStyle name="Currency 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{6A4B848D-6F0C-084D-AC60-D8831C239FEE}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -719,22 +614,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691212B9-82E4-9944-88A2-E50B4C69E4DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -748,7 +643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>0</v>
       </c>
@@ -762,7 +657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -770,7 +665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>8</v>
       </c>
@@ -788,7 +683,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -799,10 +694,10 @@
         <v>9</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -833,7 +728,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -864,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -895,7 +790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -926,7 +821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -964,319 +859,224 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210135AB-8413-D44B-BF05-443DBA342A50}">
-  <dimension ref="A1:J22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="28.83203125" style="1" customWidth="1"/>
-    <col min="3" max="11" width="8.83203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>16</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5</v>
       </c>
       <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
         <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1">
-        <v>6</v>
-      </c>
-      <c r="I6" s="1">
-        <v>7</v>
-      </c>
-      <c r="J6" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1">
-        <v>60</v>
-      </c>
-      <c r="D7" s="1">
-        <v>110</v>
-      </c>
-      <c r="E7" s="1">
-        <v>53</v>
-      </c>
-      <c r="F7" s="1">
-        <v>47</v>
-      </c>
-      <c r="G7" s="1">
-        <v>92</v>
-      </c>
-      <c r="H7" s="1">
-        <v>85</v>
-      </c>
-      <c r="I7" s="1">
-        <v>73</v>
-      </c>
-      <c r="J7" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1">
-        <v>4</v>
-      </c>
-      <c r="G8" s="1">
-        <v>7</v>
-      </c>
-      <c r="H8" s="1">
-        <v>6</v>
-      </c>
-      <c r="I8" s="1">
-        <v>8</v>
-      </c>
-      <c r="J8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1">
-        <v>82</v>
-      </c>
-      <c r="E9" s="1">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1">
-        <v>56</v>
-      </c>
-      <c r="H9" s="1">
-        <v>61</v>
-      </c>
-      <c r="I9" s="1">
-        <v>48</v>
-      </c>
-      <c r="J9" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="6">
-        <f>SUMPRODUCT(C12:J12,C9:J9)</f>
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="4">
-        <f>SUMPRODUCT(C12:J12,C7:J7)*1000</f>
-        <v>268000</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="4">
-        <f>C3</f>
-        <v>300000</v>
-      </c>
-      <c r="F19" s="1">
-        <f>E19-C19</f>
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="4">
-        <f>SUMPRODUCT(C12:J12,C8:J8)</f>
-        <v>23</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="4">
-        <v>40</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" ref="F20:F22" si="0">E20-C20</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="4">
-        <f>D12+G12</f>
-        <v>1</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="4">
-        <f>SUM(G12:J12)</f>
-        <v>2</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="4">
-        <v>2</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>